<commit_message>
Cambio de RPT al llenarlos con DataSet
</commit_message>
<xml_diff>
--- a/Maiz/Libro1.xlsx
+++ b/Maiz/Libro1.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSISTEMAS\Desktop\MAIZ A SERVER12\proyectosANH\Maiz\"/>
@@ -24,7 +24,179 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+  <si>
+    <t>COL00001</t>
+  </si>
+  <si>
+    <t>NUEVA HOLANDA</t>
+  </si>
+  <si>
+    <t>COLONIA NUEVA HOLANDA</t>
+  </si>
+  <si>
+    <t>COL00003</t>
+  </si>
+  <si>
+    <t>EL ANTEOJO</t>
+  </si>
+  <si>
+    <t>ANTEOJO JULIMES CHIH</t>
+  </si>
+  <si>
+    <t>COL00004</t>
+  </si>
+  <si>
+    <t>LOS CIENES</t>
+  </si>
+  <si>
+    <t>COLONIA LOS CIENES</t>
+  </si>
+  <si>
+    <t>COL00005</t>
+  </si>
+  <si>
+    <t>EL OASIS</t>
+  </si>
+  <si>
+    <t>COLONIA EL OASIS</t>
+  </si>
+  <si>
+    <t>COL00006</t>
+  </si>
+  <si>
+    <t>NUEVO OASIS</t>
+  </si>
+  <si>
+    <t>COLONIA NUEVO OASIS</t>
+  </si>
+  <si>
+    <t>COL00007</t>
+  </si>
+  <si>
+    <t>LAS BOMBAS</t>
+  </si>
+  <si>
+    <t>COLONIA LAS BOMBAS</t>
+  </si>
+  <si>
+    <t>COL00008</t>
+  </si>
+  <si>
+    <t>LOS JUNCOS</t>
+  </si>
+  <si>
+    <t>COLONIA LOS CUNCOS</t>
+  </si>
+  <si>
+    <t>COL00009</t>
+  </si>
+  <si>
+    <t>EL TREBOL</t>
+  </si>
+  <si>
+    <t>COLONIA EL TREBOL</t>
+  </si>
+  <si>
+    <t>COL00010</t>
+  </si>
+  <si>
+    <t>TFO</t>
+  </si>
+  <si>
+    <t>RANCHO TFO</t>
+  </si>
+  <si>
+    <t>COL00011</t>
+  </si>
+  <si>
+    <t>SAN FRANCISCO</t>
+  </si>
+  <si>
+    <t>RANCHO SAN FRANCISCO</t>
+  </si>
+  <si>
+    <t>COL00012</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LAS PALMERAS </t>
+  </si>
+  <si>
+    <t>COLONIA LAS PALMERAS</t>
+  </si>
+  <si>
+    <t>COL00013</t>
+  </si>
+  <si>
+    <t>SAN GUILLERMOS</t>
+  </si>
+  <si>
+    <t>COLONIA SAN GUILLERMO</t>
+  </si>
+  <si>
+    <t>COL00014</t>
+  </si>
+  <si>
+    <t>EL MIMBRE</t>
+  </si>
+  <si>
+    <t>COLONIA EL MIMBRE</t>
+  </si>
+  <si>
+    <t>COL00015</t>
+  </si>
+  <si>
+    <t>EL CADILLAL</t>
+  </si>
+  <si>
+    <t>COLONIA EL CADILLAL</t>
+  </si>
+  <si>
+    <t>COL00016</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOS VOLCANES </t>
+  </si>
+  <si>
+    <t>COLONIA LOS VOLCANES</t>
+  </si>
+  <si>
+    <t>COL00017</t>
+  </si>
+  <si>
+    <t>SAN ALFONSO</t>
+  </si>
+  <si>
+    <t>RANCHO SAN ALFONSO</t>
+  </si>
+  <si>
+    <t>COL00018</t>
+  </si>
+  <si>
+    <t>EL MILAGRO</t>
+  </si>
+  <si>
+    <t>COLONIA EL MILAGRO</t>
+  </si>
+  <si>
+    <t>COL00019</t>
+  </si>
+  <si>
+    <t>EL VERJEL</t>
+  </si>
+  <si>
+    <t>COLONIA EL VERJEL</t>
+  </si>
+  <si>
+    <t>COL00020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SANTA SOFIA </t>
+  </si>
+  <si>
+    <t>COLONIA SANTA SOFIA</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -374,7 +546,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B2:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
@@ -385,7 +557,274 @@
     <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>32886</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4">
+        <v>32880</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>32880</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6">
+        <v>32880</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>32886</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>32886</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9">
+        <v>32880</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10">
+        <v>32880</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11">
+        <v>32880</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12">
+        <v>32886</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13">
+        <v>32886</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14">
+        <v>32886</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15">
+        <v>32886</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16">
+        <v>32886</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E17">
+        <v>32886</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18">
+        <v>32886</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" t="s">
+        <v>53</v>
+      </c>
+      <c r="E19">
+        <v>32886</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20">
+        <v>32886</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>